<commit_message>
conflicted files when merging with master
</commit_message>
<xml_diff>
--- a/Latitude Longitude for each state.xlsx
+++ b/Latitude Longitude for each state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\project-one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4661DA78-A676-45DA-B072-0F29FA340D91}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870A7721-7F7E-4211-A781-A02D9E6EAC86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1524" yWindow="1716" windowWidth="17280" windowHeight="8964" xr2:uid="{DF66DF3A-68C3-4053-AAAE-E3DEFF05C2F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DF66DF3A-68C3-4053-AAAE-E3DEFF05C2F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>IA</t>
   </si>
   <si>
-    <t>State Abbreviations</t>
-  </si>
-  <si>
     <t>KS</t>
   </si>
   <si>
@@ -348,6 +342,12 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>State (full name)</t>
   </si>
 </sst>
 </file>
@@ -701,9 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1F9AE0-4475-4296-BED5-7C242D19BB80}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -713,24 +711,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>32.806671000000001</v>
@@ -741,10 +739,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>61.370716000000002</v>
@@ -755,10 +753,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4">
         <v>33.729759000000001</v>
@@ -769,10 +767,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>34.969704</v>
@@ -783,10 +781,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>36.116202999999999</v>
@@ -797,10 +795,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>39.059811000000003</v>
@@ -811,10 +809,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>41.597782000000002</v>
@@ -825,10 +823,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9">
         <v>39.318522999999999</v>
@@ -839,10 +837,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>38.897438000000001</v>
@@ -853,10 +851,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11">
         <v>27.766279000000001</v>
@@ -867,10 +865,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12">
         <v>33.040619</v>
@@ -881,10 +879,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13">
         <v>21.094318000000001</v>
@@ -895,10 +893,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14">
         <v>44.240459000000001</v>
@@ -909,10 +907,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15">
         <v>40.349457000000001</v>
@@ -923,10 +921,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16">
         <v>39.849426000000001</v>
@@ -937,10 +935,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17">
         <v>42.011538999999999</v>
@@ -951,10 +949,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18">
         <v>38.526600000000002</v>
@@ -965,10 +963,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C19">
         <v>37.668140000000001</v>
@@ -979,10 +977,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C20">
         <v>31.169546</v>
@@ -993,10 +991,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>44.693947000000001</v>
@@ -1007,10 +1005,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22">
         <v>39.063946000000001</v>
@@ -1021,10 +1019,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C23">
         <v>42.230170999999999</v>
@@ -1035,10 +1033,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>43.326618000000003</v>
@@ -1049,10 +1047,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25">
         <v>45.694454</v>
@@ -1063,10 +1061,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>32.741646000000003</v>
@@ -1077,10 +1075,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C27">
         <v>38.456085000000002</v>
@@ -1091,10 +1089,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28">
         <v>46.921925000000002</v>
@@ -1105,10 +1103,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C29">
         <v>41.125369999999997</v>
@@ -1119,10 +1117,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C30">
         <v>38.313515000000002</v>
@@ -1133,10 +1131,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C31">
         <v>43.452491999999999</v>
@@ -1147,10 +1145,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C32">
         <v>40.298904</v>
@@ -1161,10 +1159,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C33">
         <v>34.840515000000003</v>
@@ -1175,10 +1173,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C34">
         <v>42.165725999999999</v>
@@ -1189,10 +1187,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35">
         <v>35.630065999999999</v>
@@ -1203,10 +1201,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C36">
         <v>47.528911999999998</v>
@@ -1217,10 +1215,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37">
         <v>40.388782999999997</v>
@@ -1231,10 +1229,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38">
         <v>35.565342000000001</v>
@@ -1245,10 +1243,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C39">
         <v>44.572020999999999</v>
@@ -1259,10 +1257,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C40">
         <v>40.590752000000002</v>
@@ -1273,10 +1271,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C41">
         <v>41.680892999999998</v>
@@ -1287,10 +1285,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C42">
         <v>33.856892000000002</v>
@@ -1301,10 +1299,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C43">
         <v>44.299782</v>
@@ -1315,10 +1313,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44">
         <v>35.747844999999998</v>
@@ -1329,10 +1327,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45">
         <v>31.054487000000002</v>
@@ -1343,10 +1341,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46">
         <v>40.150032000000003</v>
@@ -1357,10 +1355,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C47">
         <v>44.045876</v>
@@ -1371,10 +1369,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48">
         <v>37.769337</v>
@@ -1385,10 +1383,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C49">
         <v>47.400902000000002</v>
@@ -1399,10 +1397,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C50">
         <v>38.491225999999997</v>
@@ -1413,10 +1411,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C51">
         <v>44.268543000000001</v>
@@ -1427,10 +1425,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C52">
         <v>42.755966000000001</v>

</xml_diff>